<commit_message>
here is the udpate there
</commit_message>
<xml_diff>
--- a/force2d/public/OccularDB_Zia.xlsx
+++ b/force2d/public/OccularDB_Zia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my data\ICAWtechnologies\Occular_dr_zia friend\Occular\Occular_force\force2d\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BD3DCD-43E3-4348-BC18-B61A8D9B0378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD203F-09E8-49B1-ACDE-BF338A856FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8BD98AE3-1540-044E-93D7-0294F8A250B2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="1235">
   <si>
     <t>EFO_Ids_Mondo</t>
   </si>
@@ -6289,9 +6289,6 @@
   </si>
   <si>
     <t>DELLEMAN SYNDROME</t>
-  </si>
-  <si>
-    <t>other</t>
   </si>
 </sst>
 </file>
@@ -6996,8 +6993,8 @@
   <dimension ref="A1:L338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E341" sqref="E341"/>
+      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E339" sqref="E339"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="16.8"/>
@@ -7156,7 +7153,7 @@
       <c r="K5" s="40"/>
       <c r="L5" s="20"/>
     </row>
-    <row r="6" spans="1:12" ht="117.6" hidden="1">
+    <row r="6" spans="1:12" ht="117.6">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -7188,7 +7185,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="117.6" hidden="1">
+    <row r="7" spans="1:12" ht="117.6">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -7298,7 +7295,7 @@
       <c r="K10" s="40"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12" hidden="1">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -7324,7 +7321,7 @@
       <c r="K11" s="40"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="1:12" hidden="1">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -7350,7 +7347,7 @@
       <c r="K12" s="40"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:12" hidden="1">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -8126,7 +8123,7 @@
       <c r="K40" s="40"/>
       <c r="L40" s="20"/>
     </row>
-    <row r="41" spans="1:12" ht="50.4" hidden="1">
+    <row r="41" spans="1:12" ht="50.4">
       <c r="A41" t="s">
         <v>126</v>
       </c>
@@ -8152,7 +8149,7 @@
       <c r="K41" s="40"/>
       <c r="L41" s="20"/>
     </row>
-    <row r="42" spans="1:12" ht="50.4" hidden="1">
+    <row r="42" spans="1:12" ht="50.4">
       <c r="A42" t="s">
         <v>126</v>
       </c>
@@ -8178,7 +8175,7 @@
       <c r="K42" s="40"/>
       <c r="L42" s="20"/>
     </row>
-    <row r="43" spans="1:12" ht="50.4" hidden="1">
+    <row r="43" spans="1:12" ht="50.4">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -8282,7 +8279,7 @@
       <c r="K46" s="40"/>
       <c r="L46" s="20"/>
     </row>
-    <row r="47" spans="1:12" ht="84" hidden="1">
+    <row r="47" spans="1:12" ht="84">
       <c r="A47" s="4" t="s">
         <v>145</v>
       </c>
@@ -8564,7 +8561,7 @@
       <c r="K57" s="40"/>
       <c r="L57" s="20"/>
     </row>
-    <row r="58" spans="1:12" hidden="1">
+    <row r="58" spans="1:12">
       <c r="A58" s="4" t="s">
         <v>181</v>
       </c>
@@ -8961,7 +8958,7 @@
       <c r="K73" s="40"/>
       <c r="L73" s="20"/>
     </row>
-    <row r="74" spans="1:12" hidden="1">
+    <row r="74" spans="1:12">
       <c r="A74" s="4" t="s">
         <v>237</v>
       </c>
@@ -8985,7 +8982,7 @@
       <c r="K74" s="40"/>
       <c r="L74" s="20"/>
     </row>
-    <row r="75" spans="1:12" ht="33.6" hidden="1">
+    <row r="75" spans="1:12" ht="33.6">
       <c r="A75" s="4" t="s">
         <v>241</v>
       </c>
@@ -9009,7 +9006,7 @@
       <c r="K75" s="40"/>
       <c r="L75" s="20"/>
     </row>
-    <row r="76" spans="1:12" hidden="1">
+    <row r="76" spans="1:12">
       <c r="A76" s="4" t="s">
         <v>245</v>
       </c>
@@ -9035,7 +9032,7 @@
       <c r="K76" s="40"/>
       <c r="L76" s="20"/>
     </row>
-    <row r="77" spans="1:12" hidden="1">
+    <row r="77" spans="1:12">
       <c r="A77" s="4" t="s">
         <v>245</v>
       </c>
@@ -9061,7 +9058,7 @@
       <c r="K77" s="40"/>
       <c r="L77" s="20"/>
     </row>
-    <row r="78" spans="1:12" hidden="1">
+    <row r="78" spans="1:12">
       <c r="A78" s="4" t="s">
         <v>245</v>
       </c>
@@ -9087,7 +9084,7 @@
       <c r="K78" s="40"/>
       <c r="L78" s="20"/>
     </row>
-    <row r="79" spans="1:12" hidden="1">
+    <row r="79" spans="1:12">
       <c r="A79" s="4" t="s">
         <v>245</v>
       </c>
@@ -9113,7 +9110,7 @@
       <c r="K79" s="40"/>
       <c r="L79" s="20"/>
     </row>
-    <row r="80" spans="1:12" hidden="1">
+    <row r="80" spans="1:12">
       <c r="C80" s="29" t="s">
         <v>249</v>
       </c>
@@ -9131,7 +9128,7 @@
       <c r="K80" s="40"/>
       <c r="L80" s="20"/>
     </row>
-    <row r="81" spans="1:12" hidden="1">
+    <row r="81" spans="1:12">
       <c r="A81" s="4" t="s">
         <v>251</v>
       </c>
@@ -9181,7 +9178,7 @@
       <c r="K82" s="40"/>
       <c r="L82" s="20"/>
     </row>
-    <row r="83" spans="1:12" ht="50.4" hidden="1">
+    <row r="83" spans="1:12" ht="50.4">
       <c r="A83" s="4" t="s">
         <v>260</v>
       </c>
@@ -9213,7 +9210,7 @@
       <c r="K83" s="40"/>
       <c r="L83" s="20"/>
     </row>
-    <row r="84" spans="1:12" ht="50.4" hidden="1">
+    <row r="84" spans="1:12" ht="50.4">
       <c r="A84" s="4" t="s">
         <v>260</v>
       </c>
@@ -9567,7 +9564,7 @@
       <c r="K95" s="40"/>
       <c r="L95" s="20"/>
     </row>
-    <row r="96" spans="1:12" ht="33.6" hidden="1">
+    <row r="96" spans="1:12" ht="33.6">
       <c r="A96" s="4" t="s">
         <v>300</v>
       </c>
@@ -9643,7 +9640,7 @@
       <c r="K98" s="40"/>
       <c r="L98" s="20"/>
     </row>
-    <row r="99" spans="1:12" ht="50.4" hidden="1">
+    <row r="99" spans="1:12" ht="50.4">
       <c r="A99" s="4" t="s">
         <v>312</v>
       </c>
@@ -10687,7 +10684,7 @@
       <c r="K138" s="40"/>
       <c r="L138" s="20"/>
     </row>
-    <row r="139" spans="1:12" ht="67.2" hidden="1">
+    <row r="139" spans="1:12" ht="67.2">
       <c r="A139" s="4" t="s">
         <v>443</v>
       </c>
@@ -10860,7 +10857,7 @@
       <c r="K145" s="40"/>
       <c r="L145" s="20"/>
     </row>
-    <row r="146" spans="1:12" ht="50.4" hidden="1">
+    <row r="146" spans="1:12" ht="50.4">
       <c r="A146" s="4" t="s">
         <v>473</v>
       </c>
@@ -11012,7 +11009,7 @@
       <c r="K151" s="40"/>
       <c r="L151" s="20"/>
     </row>
-    <row r="152" spans="1:12" ht="84" hidden="1">
+    <row r="152" spans="1:12" ht="84">
       <c r="A152" s="4" t="s">
         <v>485</v>
       </c>
@@ -11038,7 +11035,7 @@
       <c r="K152" s="40"/>
       <c r="L152" s="20"/>
     </row>
-    <row r="153" spans="1:12" ht="84" hidden="1">
+    <row r="153" spans="1:12" ht="84">
       <c r="A153" s="4" t="s">
         <v>485</v>
       </c>
@@ -11064,7 +11061,7 @@
       <c r="K153" s="40"/>
       <c r="L153" s="20"/>
     </row>
-    <row r="154" spans="1:12" ht="84" hidden="1">
+    <row r="154" spans="1:12" ht="84">
       <c r="A154" s="4" t="s">
         <v>485</v>
       </c>
@@ -11090,7 +11087,7 @@
       <c r="K154" s="40"/>
       <c r="L154" s="20"/>
     </row>
-    <row r="155" spans="1:12" ht="84" hidden="1">
+    <row r="155" spans="1:12" ht="84">
       <c r="A155" s="4" t="s">
         <v>485</v>
       </c>
@@ -11116,7 +11113,7 @@
       <c r="K155" s="40"/>
       <c r="L155" s="20"/>
     </row>
-    <row r="156" spans="1:12" ht="84" hidden="1">
+    <row r="156" spans="1:12" ht="84">
       <c r="A156" s="4" t="s">
         <v>485</v>
       </c>
@@ -11142,7 +11139,7 @@
       <c r="K156" s="40"/>
       <c r="L156" s="20"/>
     </row>
-    <row r="157" spans="1:12" ht="84" hidden="1">
+    <row r="157" spans="1:12" ht="84">
       <c r="A157" s="4" t="s">
         <v>485</v>
       </c>
@@ -12034,7 +12031,7 @@
       <c r="K191" s="40"/>
       <c r="L191" s="20"/>
     </row>
-    <row r="192" spans="1:12" ht="67.2" hidden="1">
+    <row r="192" spans="1:12" ht="67.2">
       <c r="C192" s="29" t="s">
         <v>611</v>
       </c>
@@ -12489,7 +12486,7 @@
       <c r="K209" s="43"/>
       <c r="L209" s="22"/>
     </row>
-    <row r="210" spans="1:12" ht="33.6" hidden="1">
+    <row r="210" spans="1:12" ht="33.6">
       <c r="A210" s="4" t="s">
         <v>671</v>
       </c>
@@ -12725,7 +12722,7 @@
       <c r="K217" s="40"/>
       <c r="L217" s="20"/>
     </row>
-    <row r="218" spans="1:12" hidden="1">
+    <row r="218" spans="1:12">
       <c r="A218" s="4" t="s">
         <v>692</v>
       </c>
@@ -12815,7 +12812,7 @@
       <c r="K220" s="40"/>
       <c r="L220" s="20"/>
     </row>
-    <row r="221" spans="1:12" hidden="1">
+    <row r="221" spans="1:12">
       <c r="C221" s="30" t="s">
         <v>703</v>
       </c>
@@ -12833,7 +12830,7 @@
       <c r="K221" s="40"/>
       <c r="L221" s="20"/>
     </row>
-    <row r="222" spans="1:12" ht="50.4" hidden="1">
+    <row r="222" spans="1:12" ht="50.4">
       <c r="A222" s="4" t="s">
         <v>705</v>
       </c>
@@ -12868,7 +12865,7 @@
       <c r="K223" s="40"/>
       <c r="L223" s="20"/>
     </row>
-    <row r="224" spans="1:12" hidden="1">
+    <row r="224" spans="1:12">
       <c r="A224" s="4" t="s">
         <v>709</v>
       </c>
@@ -12894,7 +12891,7 @@
       <c r="K224" s="40"/>
       <c r="L224" s="20"/>
     </row>
-    <row r="225" spans="1:12" hidden="1">
+    <row r="225" spans="1:12">
       <c r="A225" s="4" t="s">
         <v>709</v>
       </c>
@@ -12920,7 +12917,7 @@
       <c r="K225" s="40"/>
       <c r="L225" s="20"/>
     </row>
-    <row r="226" spans="1:12" hidden="1">
+    <row r="226" spans="1:12">
       <c r="A226" s="4" t="s">
         <v>709</v>
       </c>
@@ -12946,7 +12943,7 @@
       <c r="K226" s="40"/>
       <c r="L226" s="20"/>
     </row>
-    <row r="227" spans="1:12" hidden="1">
+    <row r="227" spans="1:12">
       <c r="A227" s="4" t="s">
         <v>709</v>
       </c>
@@ -12998,7 +12995,7 @@
       <c r="K228" s="40"/>
       <c r="L228" s="20"/>
     </row>
-    <row r="229" spans="1:12" ht="50.4" hidden="1">
+    <row r="229" spans="1:12" ht="50.4">
       <c r="A229" s="4" t="s">
         <v>717</v>
       </c>
@@ -13024,7 +13021,7 @@
       <c r="K229" s="40"/>
       <c r="L229" s="20"/>
     </row>
-    <row r="230" spans="1:12" ht="50.4" hidden="1">
+    <row r="230" spans="1:12" ht="50.4">
       <c r="A230" s="4" t="s">
         <v>717</v>
       </c>
@@ -13050,7 +13047,7 @@
       <c r="K230" s="40"/>
       <c r="L230" s="20"/>
     </row>
-    <row r="231" spans="1:12" ht="50.4" hidden="1">
+    <row r="231" spans="1:12" ht="50.4">
       <c r="A231" s="4" t="s">
         <v>717</v>
       </c>
@@ -13076,7 +13073,7 @@
       <c r="K231" s="40"/>
       <c r="L231" s="20"/>
     </row>
-    <row r="232" spans="1:12" ht="50.4" hidden="1">
+    <row r="232" spans="1:12" ht="50.4">
       <c r="A232" s="4" t="s">
         <v>717</v>
       </c>
@@ -13248,7 +13245,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="238" spans="1:12" hidden="1">
+    <row r="238" spans="1:12">
       <c r="A238" s="4" t="s">
         <v>740</v>
       </c>
@@ -13366,7 +13363,7 @@
       <c r="K242" s="40"/>
       <c r="L242" s="20"/>
     </row>
-    <row r="243" spans="1:12" ht="33.6" hidden="1">
+    <row r="243" spans="1:12" ht="33.6">
       <c r="A243" s="4" t="s">
         <v>755</v>
       </c>
@@ -13516,7 +13513,7 @@
       <c r="K248" s="40"/>
       <c r="L248" s="20"/>
     </row>
-    <row r="249" spans="1:12" hidden="1">
+    <row r="249" spans="1:12">
       <c r="A249" s="4" t="s">
         <v>775</v>
       </c>
@@ -13540,7 +13537,7 @@
       <c r="K249" s="40"/>
       <c r="L249" s="20"/>
     </row>
-    <row r="250" spans="1:12" ht="67.2" hidden="1">
+    <row r="250" spans="1:12" ht="67.2">
       <c r="A250" s="4" t="s">
         <v>779</v>
       </c>
@@ -13566,7 +13563,7 @@
       <c r="K250" s="40"/>
       <c r="L250" s="20"/>
     </row>
-    <row r="251" spans="1:12" ht="50.4" hidden="1">
+    <row r="251" spans="1:12" ht="50.4">
       <c r="A251" s="4" t="s">
         <v>784</v>
       </c>
@@ -13665,7 +13662,7 @@
       <c r="K254" s="40"/>
       <c r="L254" s="20"/>
     </row>
-    <row r="255" spans="1:12" hidden="1">
+    <row r="255" spans="1:12">
       <c r="A255" s="4" t="s">
         <v>796</v>
       </c>
@@ -13948,7 +13945,7 @@
       <c r="K265" s="40"/>
       <c r="L265" s="20"/>
     </row>
-    <row r="266" spans="1:12" hidden="1">
+    <row r="266" spans="1:12">
       <c r="A266" s="4" t="s">
         <v>822</v>
       </c>
@@ -13974,7 +13971,7 @@
       <c r="K266" s="40"/>
       <c r="L266" s="20"/>
     </row>
-    <row r="267" spans="1:12" hidden="1">
+    <row r="267" spans="1:12">
       <c r="A267" s="4" t="s">
         <v>822</v>
       </c>
@@ -14000,7 +13997,7 @@
       <c r="K267" s="40"/>
       <c r="L267" s="20"/>
     </row>
-    <row r="268" spans="1:12" hidden="1">
+    <row r="268" spans="1:12">
       <c r="A268" s="4" t="s">
         <v>822</v>
       </c>
@@ -14312,7 +14309,7 @@
       <c r="K278" s="40"/>
       <c r="L278" s="20"/>
     </row>
-    <row r="279" spans="1:12" hidden="1">
+    <row r="279" spans="1:12">
       <c r="C279" s="29" t="s">
         <v>852</v>
       </c>
@@ -14350,7 +14347,7 @@
       <c r="K280" s="40"/>
       <c r="L280" s="20"/>
     </row>
-    <row r="281" spans="1:12" ht="67.2" hidden="1">
+    <row r="281" spans="1:12" ht="67.2">
       <c r="A281" s="4" t="s">
         <v>856</v>
       </c>
@@ -14376,7 +14373,7 @@
       <c r="K281" s="40"/>
       <c r="L281" s="20"/>
     </row>
-    <row r="282" spans="1:12" ht="67.2" hidden="1">
+    <row r="282" spans="1:12" ht="67.2">
       <c r="A282" s="4" t="s">
         <v>856</v>
       </c>
@@ -14402,7 +14399,7 @@
       <c r="K282" s="40"/>
       <c r="L282" s="20"/>
     </row>
-    <row r="283" spans="1:12" ht="67.2" hidden="1">
+    <row r="283" spans="1:12" ht="67.2">
       <c r="A283" s="4" t="s">
         <v>856</v>
       </c>
@@ -14428,7 +14425,7 @@
       <c r="K283" s="40"/>
       <c r="L283" s="20"/>
     </row>
-    <row r="284" spans="1:12" ht="50.4" hidden="1">
+    <row r="284" spans="1:12" ht="50.4">
       <c r="A284" s="4" t="s">
         <v>740</v>
       </c>
@@ -14454,7 +14451,7 @@
       <c r="K284" s="40"/>
       <c r="L284" s="20"/>
     </row>
-    <row r="285" spans="1:12" ht="50.4" hidden="1">
+    <row r="285" spans="1:12" ht="50.4">
       <c r="A285" s="4" t="s">
         <v>740</v>
       </c>
@@ -14480,7 +14477,7 @@
       <c r="K285" s="40"/>
       <c r="L285" s="20"/>
     </row>
-    <row r="286" spans="1:12" ht="50.4" hidden="1">
+    <row r="286" spans="1:12" ht="50.4">
       <c r="A286" s="4" t="s">
         <v>740</v>
       </c>
@@ -14506,7 +14503,7 @@
       <c r="K286" s="40"/>
       <c r="L286" s="20"/>
     </row>
-    <row r="287" spans="1:12" ht="50.4" hidden="1">
+    <row r="287" spans="1:12" ht="50.4">
       <c r="A287" s="4" t="s">
         <v>740</v>
       </c>
@@ -14532,7 +14529,7 @@
       <c r="K287" s="40"/>
       <c r="L287" s="20"/>
     </row>
-    <row r="288" spans="1:12" ht="50.4" hidden="1">
+    <row r="288" spans="1:12" ht="50.4">
       <c r="A288" s="4" t="s">
         <v>740</v>
       </c>
@@ -14558,7 +14555,7 @@
       <c r="K288" s="40"/>
       <c r="L288" s="20"/>
     </row>
-    <row r="289" spans="1:12" hidden="1">
+    <row r="289" spans="1:12">
       <c r="A289" s="4" t="s">
         <v>862</v>
       </c>
@@ -14702,7 +14699,7 @@
         <v>886</v>
       </c>
       <c r="E294" s="4" t="s">
-        <v>1235</v>
+        <v>1020</v>
       </c>
       <c r="F294" s="25"/>
       <c r="G294" s="6"/>
@@ -15018,7 +15015,7 @@
       <c r="K307" s="40"/>
       <c r="L307" s="20"/>
     </row>
-    <row r="308" spans="1:12" ht="33.6" hidden="1">
+    <row r="308" spans="1:12" ht="33.6">
       <c r="A308" s="4" t="s">
         <v>936</v>
       </c>
@@ -15042,7 +15039,7 @@
       <c r="K308" s="40"/>
       <c r="L308" s="20"/>
     </row>
-    <row r="309" spans="1:12" ht="33.6" hidden="1">
+    <row r="309" spans="1:12" ht="33.6">
       <c r="A309" s="4" t="s">
         <v>940</v>
       </c>
@@ -15068,7 +15065,7 @@
       <c r="K309" s="40"/>
       <c r="L309" s="20"/>
     </row>
-    <row r="310" spans="1:12" ht="33.6" hidden="1">
+    <row r="310" spans="1:12" ht="33.6">
       <c r="A310" s="4" t="s">
         <v>940</v>
       </c>
@@ -15094,7 +15091,7 @@
       <c r="K310" s="40"/>
       <c r="L310" s="20"/>
     </row>
-    <row r="311" spans="1:12" ht="50.4" hidden="1">
+    <row r="311" spans="1:12" ht="50.4">
       <c r="A311" s="4" t="s">
         <v>944</v>
       </c>
@@ -15170,7 +15167,7 @@
       <c r="K313" s="40"/>
       <c r="L313" s="20"/>
     </row>
-    <row r="314" spans="1:12" ht="33.6" hidden="1">
+    <row r="314" spans="1:12" ht="33.6">
       <c r="A314" s="4" t="s">
         <v>958</v>
       </c>
@@ -15298,7 +15295,7 @@
       <c r="K318" s="40"/>
       <c r="L318" s="20"/>
     </row>
-    <row r="319" spans="1:12" hidden="1">
+    <row r="319" spans="1:12">
       <c r="A319" s="4" t="s">
         <v>976</v>
       </c>
@@ -15320,7 +15317,7 @@
       <c r="K319" s="40"/>
       <c r="L319" s="20"/>
     </row>
-    <row r="320" spans="1:12" hidden="1">
+    <row r="320" spans="1:12">
       <c r="A320" s="4" t="s">
         <v>976</v>
       </c>
@@ -15352,7 +15349,7 @@
       <c r="K320" s="40"/>
       <c r="L320" s="20"/>
     </row>
-    <row r="321" spans="1:12" hidden="1">
+    <row r="321" spans="1:12">
       <c r="A321" s="4" t="s">
         <v>976</v>
       </c>
@@ -15378,7 +15375,7 @@
       <c r="K321" s="40"/>
       <c r="L321" s="20"/>
     </row>
-    <row r="322" spans="1:12" hidden="1">
+    <row r="322" spans="1:12">
       <c r="A322" s="4" t="s">
         <v>976</v>
       </c>
@@ -15404,7 +15401,7 @@
       <c r="K322" s="40"/>
       <c r="L322" s="20"/>
     </row>
-    <row r="323" spans="1:12" hidden="1">
+    <row r="323" spans="1:12">
       <c r="A323" s="4" t="s">
         <v>976</v>
       </c>
@@ -15430,7 +15427,7 @@
       <c r="K323" s="40"/>
       <c r="L323" s="20"/>
     </row>
-    <row r="324" spans="1:12" hidden="1">
+    <row r="324" spans="1:12">
       <c r="A324" s="4" t="s">
         <v>976</v>
       </c>
@@ -15508,7 +15505,7 @@
       <c r="K326" s="40"/>
       <c r="L326" s="20"/>
     </row>
-    <row r="327" spans="1:12" ht="50.4" hidden="1">
+    <row r="327" spans="1:12" ht="50.4">
       <c r="A327" s="4" t="s">
         <v>989</v>
       </c>
@@ -15534,7 +15531,7 @@
       <c r="K327" s="40"/>
       <c r="L327" s="20"/>
     </row>
-    <row r="328" spans="1:12" ht="50.4" hidden="1">
+    <row r="328" spans="1:12" ht="50.4">
       <c r="A328" s="4" t="s">
         <v>989</v>
       </c>
@@ -15560,7 +15557,7 @@
       <c r="K328" s="40"/>
       <c r="L328" s="20"/>
     </row>
-    <row r="329" spans="1:12" ht="50.4" hidden="1">
+    <row r="329" spans="1:12" ht="50.4">
       <c r="A329" s="4" t="s">
         <v>989</v>
       </c>
@@ -15823,7 +15820,7 @@
   <autoFilter ref="E1:E338" xr:uid="{400770C2-249E-0F45-890C-AF972D0CDD11}">
     <filterColumn colId="0">
       <filters>
-        <filter val="X-linked"/>
+        <filter val="Other"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
udpate the data there
</commit_message>
<xml_diff>
--- a/force2d/public/OccularDB_Zia.xlsx
+++ b/force2d/public/OccularDB_Zia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\my data\ICAWtechnologies\Occular_dr_zia friend\Occular\Occular_force\force2d\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BBD203F-09E8-49B1-ACDE-BF338A856FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0832F357-B998-4694-9AB5-9CC31E7E8155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8BD98AE3-1540-044E-93D7-0294F8A250B2}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="1235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="1234">
   <si>
     <t>EFO_Ids_Mondo</t>
   </si>
@@ -5650,9 +5650,6 @@
   </si>
   <si>
     <t>Autosomal recessive</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> X-linked dominant</t>
   </si>
   <si>
     <t>Autosomal dominant</t>
@@ -6993,8 +6990,8 @@
   <dimension ref="A1:L338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A294" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E339" sqref="E339"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="16.8"/>
@@ -7003,7 +7000,7 @@
     <col min="2" max="2" width="17.69921875" customWidth="1"/>
     <col min="3" max="3" width="35" style="29" customWidth="1"/>
     <col min="4" max="4" width="36.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.69921875" customWidth="1"/>
+    <col min="5" max="5" width="28.296875" customWidth="1"/>
     <col min="6" max="6" width="11.69921875" style="27" customWidth="1"/>
     <col min="7" max="7" width="12.296875" customWidth="1"/>
     <col min="8" max="8" width="13.296875" customWidth="1"/>
@@ -7036,13 +7033,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="I1" s="32" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="K1" s="39" t="s">
         <v>8</v>
@@ -7094,7 +7091,7 @@
         <v>1021</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -7120,7 +7117,7 @@
         <v>1021</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -7129,7 +7126,7 @@
       <c r="K4" s="40"/>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="1:12" ht="67.2" hidden="1">
+    <row r="5" spans="1:12" ht="67.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -7143,7 +7140,7 @@
         <v>22</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="F5" s="25"/>
       <c r="G5" s="6"/>
@@ -7153,7 +7150,7 @@
       <c r="K5" s="40"/>
       <c r="L5" s="20"/>
     </row>
-    <row r="6" spans="1:12" ht="117.6">
+    <row r="6" spans="1:12" ht="117.6" hidden="1">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -7170,13 +7167,13 @@
         <v>1020</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="35"/>
       <c r="J6" s="18" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="K6" s="41" t="s">
         <v>28</v>
@@ -7185,7 +7182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="117.6">
+    <row r="7" spans="1:12" ht="117.6" hidden="1">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -7202,13 +7199,13 @@
         <v>1020</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="35"/>
       <c r="J7" s="18" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="K7" s="41" t="s">
         <v>28</v>
@@ -7243,7 +7240,7 @@
       <c r="K8" s="40"/>
       <c r="L8" s="20"/>
     </row>
-    <row r="9" spans="1:12" ht="33.6" hidden="1">
+    <row r="9" spans="1:12" ht="33.6">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -7257,7 +7254,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>39</v>
@@ -7295,7 +7292,7 @@
       <c r="K10" s="40"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" hidden="1">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -7312,7 +7309,7 @@
         <v>1020</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
@@ -7321,7 +7318,7 @@
       <c r="K11" s="40"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" hidden="1">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -7338,7 +7335,7 @@
         <v>1020</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
@@ -7347,7 +7344,7 @@
       <c r="K12" s="40"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" hidden="1">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -7364,7 +7361,7 @@
         <v>1020</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
@@ -7416,19 +7413,19 @@
         <v>58</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="35"/>
       <c r="J15" s="18" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="K15" s="41" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="L15" s="21" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="33.6" hidden="1">
@@ -7448,19 +7445,19 @@
         <v>58</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="35"/>
       <c r="J16" s="18" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="K16" s="41" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="33.6" hidden="1">
@@ -7480,19 +7477,19 @@
         <v>58</v>
       </c>
       <c r="F17" s="24" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="35"/>
       <c r="J17" s="18" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="K17" s="41" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="33.6" hidden="1">
@@ -7512,19 +7509,19 @@
         <v>58</v>
       </c>
       <c r="F18" s="24" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="35"/>
       <c r="J18" s="18" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="K18" s="41" t="s">
+        <v>1171</v>
+      </c>
+      <c r="L18" s="21" t="s">
         <v>1172</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="33.6" hidden="1">
@@ -7544,19 +7541,19 @@
         <v>58</v>
       </c>
       <c r="F19" s="24" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="35"/>
       <c r="J19" s="18" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="K19" s="41" t="s">
+        <v>1171</v>
+      </c>
+      <c r="L19" s="21" t="s">
         <v>1172</v>
-      </c>
-      <c r="L19" s="21" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="33.6" hidden="1">
@@ -7576,19 +7573,19 @@
         <v>58</v>
       </c>
       <c r="F20" s="24" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="35"/>
       <c r="J20" s="18" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="K20" s="41" t="s">
+        <v>1171</v>
+      </c>
+      <c r="L20" s="21" t="s">
         <v>1172</v>
-      </c>
-      <c r="L20" s="21" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="33.6" hidden="1">
@@ -7605,10 +7602,10 @@
         <v>62</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F21" s="24" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G21" s="6"/>
       <c r="H21" s="6"/>
@@ -7631,10 +7628,10 @@
         <v>62</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F22" s="24" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
@@ -7657,10 +7654,10 @@
         <v>66</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F23" s="24" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
@@ -7683,10 +7680,10 @@
         <v>66</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
@@ -7709,19 +7706,19 @@
         <v>70</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>71</v>
       </c>
       <c r="G25" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>1174</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="I25" s="33" t="s">
         <v>1175</v>
-      </c>
-      <c r="I25" s="33" t="s">
-        <v>1176</v>
       </c>
       <c r="J25" s="7"/>
       <c r="K25" s="40"/>
@@ -7783,7 +7780,7 @@
         <v>81</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>82</v>
@@ -7867,19 +7864,19 @@
         <v>97</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>98</v>
       </c>
       <c r="G31" s="6" t="s">
+        <v>1184</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>1185</v>
       </c>
-      <c r="H31" s="6" t="s">
-        <v>1186</v>
-      </c>
       <c r="I31" s="33" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J31" s="7"/>
       <c r="K31" s="40"/>
@@ -7899,7 +7896,7 @@
         <v>102</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F32" s="24" t="s">
         <v>103</v>
@@ -7925,10 +7922,10 @@
         <v>107</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
@@ -7951,10 +7948,10 @@
         <v>107</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
@@ -7977,7 +7974,7 @@
         <v>111</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>112</v>
@@ -8027,10 +8024,10 @@
         <v>121</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
@@ -8053,10 +8050,10 @@
         <v>121</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
@@ -8079,10 +8076,10 @@
         <v>121</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F39" s="24" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
@@ -8105,25 +8102,25 @@
         <v>125</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F40" s="24" t="s">
         <v>71</v>
       </c>
       <c r="G40" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>1174</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="I40" s="33" t="s">
         <v>1175</v>
-      </c>
-      <c r="I40" s="33" t="s">
-        <v>1176</v>
       </c>
       <c r="J40" s="7"/>
       <c r="K40" s="40"/>
       <c r="L40" s="20"/>
     </row>
-    <row r="41" spans="1:12" ht="50.4">
+    <row r="41" spans="1:12" ht="50.4" hidden="1">
       <c r="A41" t="s">
         <v>126</v>
       </c>
@@ -8140,7 +8137,7 @@
         <v>1020</v>
       </c>
       <c r="F41" s="24" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
@@ -8149,7 +8146,7 @@
       <c r="K41" s="40"/>
       <c r="L41" s="20"/>
     </row>
-    <row r="42" spans="1:12" ht="50.4">
+    <row r="42" spans="1:12" ht="50.4" hidden="1">
       <c r="A42" t="s">
         <v>126</v>
       </c>
@@ -8166,7 +8163,7 @@
         <v>1020</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
@@ -8175,7 +8172,7 @@
       <c r="K42" s="40"/>
       <c r="L42" s="20"/>
     </row>
-    <row r="43" spans="1:12" ht="50.4">
+    <row r="43" spans="1:12" ht="50.4" hidden="1">
       <c r="A43" t="s">
         <v>126</v>
       </c>
@@ -8192,7 +8189,7 @@
         <v>1020</v>
       </c>
       <c r="F43" s="24" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
@@ -8215,7 +8212,7 @@
         <v>133</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>134</v>
@@ -8267,7 +8264,7 @@
         <v>143</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>144</v>
@@ -8279,7 +8276,7 @@
       <c r="K46" s="40"/>
       <c r="L46" s="20"/>
     </row>
-    <row r="47" spans="1:12" ht="84">
+    <row r="47" spans="1:12" ht="84" hidden="1">
       <c r="A47" s="4" t="s">
         <v>145</v>
       </c>
@@ -8371,10 +8368,10 @@
         <v>157</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F50" s="24" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
@@ -8397,10 +8394,10 @@
         <v>157</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
@@ -8423,10 +8420,10 @@
         <v>157</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F52" s="24" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
@@ -8449,7 +8446,7 @@
         <v>161</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F53" s="24" t="s">
         <v>162</v>
@@ -8525,7 +8522,7 @@
         <v>175</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F56" s="25"/>
       <c r="G56" s="6"/>
@@ -8561,7 +8558,7 @@
       <c r="K57" s="40"/>
       <c r="L57" s="20"/>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" hidden="1">
       <c r="A58" s="4" t="s">
         <v>181</v>
       </c>
@@ -8599,10 +8596,10 @@
         <v>188</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
@@ -8625,10 +8622,10 @@
         <v>188</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F60" s="24" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
@@ -8677,7 +8674,7 @@
         <v>197</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F62" s="24" t="s">
         <v>198</v>
@@ -8689,7 +8686,7 @@
       <c r="K62" s="40"/>
       <c r="L62" s="20"/>
     </row>
-    <row r="63" spans="1:12" ht="33.6" hidden="1">
+    <row r="63" spans="1:12" ht="33.6">
       <c r="A63" s="4" t="s">
         <v>200</v>
       </c>
@@ -8703,7 +8700,7 @@
         <v>203</v>
       </c>
       <c r="E63" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F63" s="24" t="s">
         <v>204</v>
@@ -8715,7 +8712,7 @@
       <c r="K63" s="40"/>
       <c r="L63" s="20"/>
     </row>
-    <row r="64" spans="1:12" hidden="1">
+    <row r="64" spans="1:12">
       <c r="A64" s="4" t="s">
         <v>205</v>
       </c>
@@ -8729,7 +8726,7 @@
         <v>208</v>
       </c>
       <c r="E64" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F64" s="25"/>
       <c r="G64" s="6"/>
@@ -8739,7 +8736,7 @@
       <c r="K64" s="40"/>
       <c r="L64" s="20"/>
     </row>
-    <row r="65" spans="1:12" ht="33.6" hidden="1">
+    <row r="65" spans="1:12" ht="33.6">
       <c r="A65" s="4" t="s">
         <v>209</v>
       </c>
@@ -8753,7 +8750,7 @@
         <v>212</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F65" s="24" t="s">
         <v>213</v>
@@ -8831,7 +8828,7 @@
         <v>1021</v>
       </c>
       <c r="F68" s="24" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
@@ -8854,10 +8851,10 @@
         <v>225</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -8880,10 +8877,10 @@
         <v>225</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F70" s="24" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
@@ -8892,7 +8889,7 @@
       <c r="K70" s="40"/>
       <c r="L70" s="20"/>
     </row>
-    <row r="71" spans="1:12" hidden="1">
+    <row r="71" spans="1:12">
       <c r="C71" s="29" t="s">
         <v>226</v>
       </c>
@@ -8900,7 +8897,7 @@
         <v>227</v>
       </c>
       <c r="E71" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F71" s="24" t="s">
         <v>228</v>
@@ -8912,7 +8909,7 @@
       <c r="K71" s="40"/>
       <c r="L71" s="20"/>
     </row>
-    <row r="72" spans="1:12" hidden="1">
+    <row r="72" spans="1:12">
       <c r="C72" s="29" t="s">
         <v>229</v>
       </c>
@@ -8920,7 +8917,7 @@
         <v>230</v>
       </c>
       <c r="E72" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F72" s="24" t="s">
         <v>231</v>
@@ -8946,7 +8943,7 @@
         <v>235</v>
       </c>
       <c r="E73" s="16" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F73" s="24" t="s">
         <v>236</v>
@@ -8958,7 +8955,7 @@
       <c r="K73" s="40"/>
       <c r="L73" s="20"/>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" hidden="1">
       <c r="A74" s="4" t="s">
         <v>237</v>
       </c>
@@ -8982,7 +8979,7 @@
       <c r="K74" s="40"/>
       <c r="L74" s="20"/>
     </row>
-    <row r="75" spans="1:12" ht="33.6">
+    <row r="75" spans="1:12" ht="33.6" hidden="1">
       <c r="A75" s="4" t="s">
         <v>241</v>
       </c>
@@ -9006,7 +9003,7 @@
       <c r="K75" s="40"/>
       <c r="L75" s="20"/>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" hidden="1">
       <c r="A76" s="4" t="s">
         <v>245</v>
       </c>
@@ -9023,7 +9020,7 @@
         <v>1020</v>
       </c>
       <c r="F76" s="24" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
@@ -9032,7 +9029,7 @@
       <c r="K76" s="40"/>
       <c r="L76" s="20"/>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" hidden="1">
       <c r="A77" s="4" t="s">
         <v>245</v>
       </c>
@@ -9049,7 +9046,7 @@
         <v>1020</v>
       </c>
       <c r="F77" s="24" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
@@ -9058,7 +9055,7 @@
       <c r="K77" s="40"/>
       <c r="L77" s="20"/>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" hidden="1">
       <c r="A78" s="4" t="s">
         <v>245</v>
       </c>
@@ -9075,7 +9072,7 @@
         <v>1020</v>
       </c>
       <c r="F78" s="24" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
@@ -9084,7 +9081,7 @@
       <c r="K78" s="40"/>
       <c r="L78" s="20"/>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" hidden="1">
       <c r="A79" s="4" t="s">
         <v>245</v>
       </c>
@@ -9101,7 +9098,7 @@
         <v>1020</v>
       </c>
       <c r="F79" s="24" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
@@ -9110,7 +9107,7 @@
       <c r="K79" s="40"/>
       <c r="L79" s="20"/>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" hidden="1">
       <c r="C80" s="29" t="s">
         <v>249</v>
       </c>
@@ -9128,7 +9125,7 @@
       <c r="K80" s="40"/>
       <c r="L80" s="20"/>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" hidden="1">
       <c r="A81" s="4" t="s">
         <v>251</v>
       </c>
@@ -9178,7 +9175,7 @@
       <c r="K82" s="40"/>
       <c r="L82" s="20"/>
     </row>
-    <row r="83" spans="1:12" ht="50.4">
+    <row r="83" spans="1:12" ht="50.4" hidden="1">
       <c r="A83" s="4" t="s">
         <v>260</v>
       </c>
@@ -9195,22 +9192,22 @@
         <v>1020</v>
       </c>
       <c r="F83" s="24" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G83" s="6" t="s">
+        <v>1176</v>
+      </c>
+      <c r="H83" s="6" t="s">
         <v>1177</v>
       </c>
-      <c r="H83" s="6" t="s">
+      <c r="I83" s="33" t="s">
         <v>1178</v>
-      </c>
-      <c r="I83" s="33" t="s">
-        <v>1179</v>
       </c>
       <c r="J83" s="7"/>
       <c r="K83" s="40"/>
       <c r="L83" s="20"/>
     </row>
-    <row r="84" spans="1:12" ht="50.4">
+    <row r="84" spans="1:12" ht="50.4" hidden="1">
       <c r="A84" s="4" t="s">
         <v>260</v>
       </c>
@@ -9227,16 +9224,16 @@
         <v>1020</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="I84" s="33" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="J84" s="7"/>
       <c r="K84" s="40"/>
@@ -9250,7 +9247,7 @@
         <v>265</v>
       </c>
       <c r="C85" s="29" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D85" s="4" t="s">
         <v>266</v>
@@ -9334,19 +9331,19 @@
         <v>280</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F88" s="24" t="s">
         <v>71</v>
       </c>
       <c r="G88" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H88" s="6" t="s">
         <v>1174</v>
       </c>
-      <c r="H88" s="6" t="s">
+      <c r="I88" s="33" t="s">
         <v>1175</v>
-      </c>
-      <c r="I88" s="33" t="s">
-        <v>1176</v>
       </c>
       <c r="J88" s="7"/>
       <c r="K88" s="40"/>
@@ -9360,25 +9357,25 @@
         <v>282</v>
       </c>
       <c r="C89" s="29" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>280</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F89" s="24" t="s">
         <v>283</v>
       </c>
       <c r="G89" s="6" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I89" s="33" t="s">
         <v>1181</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>1183</v>
-      </c>
-      <c r="I89" s="33" t="s">
-        <v>1182</v>
       </c>
       <c r="J89" s="7"/>
       <c r="K89" s="40"/>
@@ -9398,19 +9395,19 @@
         <v>280</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F90" s="24" t="s">
         <v>71</v>
       </c>
       <c r="G90" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H90" s="6" t="s">
         <v>1174</v>
       </c>
-      <c r="H90" s="6" t="s">
+      <c r="I90" s="33" t="s">
         <v>1175</v>
-      </c>
-      <c r="I90" s="33" t="s">
-        <v>1176</v>
       </c>
       <c r="J90" s="7"/>
       <c r="K90" s="40"/>
@@ -9424,25 +9421,25 @@
         <v>282</v>
       </c>
       <c r="C91" s="29" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D91" s="4" t="s">
         <v>280</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F91" s="24" t="s">
         <v>283</v>
       </c>
       <c r="G91" s="6" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I91" s="33" t="s">
         <v>1181</v>
-      </c>
-      <c r="H91" s="6" t="s">
-        <v>1183</v>
-      </c>
-      <c r="I91" s="33" t="s">
-        <v>1182</v>
       </c>
       <c r="J91" s="7"/>
       <c r="K91" s="40"/>
@@ -9497,13 +9494,13 @@
       <c r="H93" s="11"/>
       <c r="I93" s="34"/>
       <c r="J93" s="18" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="K93" s="41" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="L93" s="20" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="94" spans="1:12" ht="18.600000000000001" hidden="1">
@@ -9529,13 +9526,13 @@
       <c r="H94" s="11"/>
       <c r="I94" s="34"/>
       <c r="J94" s="18" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="K94" s="41" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="L94" s="20" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="95" spans="1:12" ht="50.4" hidden="1">
@@ -9564,7 +9561,7 @@
       <c r="K95" s="40"/>
       <c r="L95" s="20"/>
     </row>
-    <row r="96" spans="1:12" ht="33.6">
+    <row r="96" spans="1:12" ht="33.6" hidden="1">
       <c r="A96" s="4" t="s">
         <v>300</v>
       </c>
@@ -9572,7 +9569,7 @@
         <v>301</v>
       </c>
       <c r="C96" s="29" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="D96" s="4" t="s">
         <v>302</v>
@@ -9596,13 +9593,13 @@
         <v>304</v>
       </c>
       <c r="C97" s="30" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>305</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F97" s="24" t="s">
         <v>306</v>
@@ -9628,7 +9625,7 @@
         <v>310</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F98" s="24" t="s">
         <v>311</v>
@@ -9640,7 +9637,7 @@
       <c r="K98" s="40"/>
       <c r="L98" s="20"/>
     </row>
-    <row r="99" spans="1:12" ht="50.4">
+    <row r="99" spans="1:12" ht="50.4" hidden="1">
       <c r="A99" s="4" t="s">
         <v>312</v>
       </c>
@@ -9704,7 +9701,7 @@
         <v>324</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F101" s="24" t="s">
         <v>325</v>
@@ -9756,10 +9753,10 @@
         <v>331</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F103" s="24" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G103" s="6"/>
       <c r="H103" s="6"/>
@@ -9782,10 +9779,10 @@
         <v>331</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F104" s="24" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="G104" s="6"/>
       <c r="H104" s="6"/>
@@ -9808,10 +9805,10 @@
         <v>331</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F105" s="24" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="G105" s="6"/>
       <c r="H105" s="6"/>
@@ -9834,10 +9831,10 @@
         <v>331</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F106" s="24" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="G106" s="6"/>
       <c r="H106" s="6"/>
@@ -9886,7 +9883,7 @@
         <v>340</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F108" s="24" t="s">
         <v>103</v>
@@ -9898,7 +9895,7 @@
       <c r="K108" s="40"/>
       <c r="L108" s="20"/>
     </row>
-    <row r="109" spans="1:12" ht="18.600000000000001" hidden="1">
+    <row r="109" spans="1:12" ht="18.600000000000001">
       <c r="A109" s="4" t="s">
         <v>341</v>
       </c>
@@ -9906,13 +9903,13 @@
         <v>342</v>
       </c>
       <c r="C109" s="30" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D109" t="s">
         <v>343</v>
       </c>
       <c r="E109" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F109" s="24" t="s">
         <v>344</v>
@@ -9921,7 +9918,7 @@
       <c r="H109" s="11"/>
       <c r="I109" s="33"/>
       <c r="J109" s="18" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="K109" s="41" t="s">
         <v>345</v>
@@ -9996,7 +9993,7 @@
         <v>360</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F112" s="24"/>
       <c r="G112" s="6"/>
@@ -10081,13 +10078,13 @@
       <c r="H115" s="11"/>
       <c r="I115" s="34"/>
       <c r="J115" s="18" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="K115" s="41" t="s">
+        <v>1192</v>
+      </c>
+      <c r="L115" s="20" t="s">
         <v>1193</v>
-      </c>
-      <c r="L115" s="20" t="s">
-        <v>1194</v>
       </c>
     </row>
     <row r="116" spans="1:12" ht="117.6" hidden="1">
@@ -10113,13 +10110,13 @@
       <c r="H116" s="11"/>
       <c r="I116" s="34"/>
       <c r="J116" s="18" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="K116" s="41" t="s">
+        <v>1194</v>
+      </c>
+      <c r="L116" s="20" t="s">
         <v>1195</v>
-      </c>
-      <c r="L116" s="20" t="s">
-        <v>1196</v>
       </c>
     </row>
     <row r="117" spans="1:12" hidden="1">
@@ -10139,7 +10136,7 @@
         <v>1021</v>
       </c>
       <c r="F117" s="24" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G117" s="6"/>
       <c r="H117" s="6"/>
@@ -10165,7 +10162,7 @@
         <v>1021</v>
       </c>
       <c r="F118" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G118" s="6"/>
       <c r="H118" s="6"/>
@@ -10188,10 +10185,10 @@
         <v>381</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F119" s="24" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G119" s="6"/>
       <c r="H119" s="6"/>
@@ -10214,10 +10211,10 @@
         <v>381</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F120" s="24" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G120" s="6"/>
       <c r="H120" s="6"/>
@@ -10234,10 +10231,10 @@
         <v>381</v>
       </c>
       <c r="E121" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F121" s="24" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G121" s="6"/>
       <c r="H121" s="6"/>
@@ -10254,10 +10251,10 @@
         <v>381</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F122" s="24" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="G122" s="6"/>
       <c r="H122" s="6"/>
@@ -10274,10 +10271,10 @@
         <v>381</v>
       </c>
       <c r="E123" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F123" s="24" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="G123" s="6"/>
       <c r="H123" s="6"/>
@@ -10372,13 +10369,13 @@
         <v>396</v>
       </c>
       <c r="C127" s="30" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="D127" t="s">
         <v>397</v>
       </c>
       <c r="E127" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F127" s="25"/>
       <c r="G127" s="6"/>
@@ -10388,7 +10385,7 @@
       <c r="K127" s="40"/>
       <c r="L127" s="20"/>
     </row>
-    <row r="128" spans="1:12" ht="50.4" hidden="1">
+    <row r="128" spans="1:12" ht="50.4">
       <c r="A128" s="4" t="s">
         <v>398</v>
       </c>
@@ -10402,7 +10399,7 @@
         <v>401</v>
       </c>
       <c r="E128" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F128" s="24" t="s">
         <v>402</v>
@@ -10428,7 +10425,7 @@
         <v>406</v>
       </c>
       <c r="E129" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F129" s="24" t="s">
         <v>103</v>
@@ -10474,13 +10471,13 @@
         <v>413</v>
       </c>
       <c r="C131" s="30" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D131" s="4" t="s">
         <v>414</v>
       </c>
       <c r="E131" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F131" s="24" t="s">
         <v>415</v>
@@ -10568,7 +10565,7 @@
       <c r="K134" s="40"/>
       <c r="L134" s="20"/>
     </row>
-    <row r="135" spans="1:12" ht="50.4" hidden="1">
+    <row r="135" spans="1:12" ht="50.4">
       <c r="A135" s="4" t="s">
         <v>430</v>
       </c>
@@ -10576,13 +10573,13 @@
         <v>431</v>
       </c>
       <c r="C135" s="30" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D135" s="4" t="s">
         <v>432</v>
       </c>
       <c r="E135" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F135" s="24" t="s">
         <v>433</v>
@@ -10608,19 +10605,19 @@
         <v>437</v>
       </c>
       <c r="E136" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F136" s="24" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G136" s="6" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H136" s="6" t="s">
         <v>1197</v>
       </c>
-      <c r="H136" s="6" t="s">
+      <c r="I136" s="33" t="s">
         <v>1198</v>
-      </c>
-      <c r="I136" s="33" t="s">
-        <v>1199</v>
       </c>
       <c r="J136" s="7"/>
       <c r="K136" s="40"/>
@@ -10640,19 +10637,19 @@
         <v>437</v>
       </c>
       <c r="E137" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F137" s="24" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G137" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H137" s="6" t="s">
         <v>1174</v>
       </c>
-      <c r="H137" s="6" t="s">
+      <c r="I137" s="33" t="s">
         <v>1175</v>
-      </c>
-      <c r="I137" s="33" t="s">
-        <v>1176</v>
       </c>
       <c r="J137" s="7"/>
       <c r="K137" s="40"/>
@@ -10684,7 +10681,7 @@
       <c r="K138" s="40"/>
       <c r="L138" s="20"/>
     </row>
-    <row r="139" spans="1:12" ht="67.2">
+    <row r="139" spans="1:12" ht="67.2" hidden="1">
       <c r="A139" s="4" t="s">
         <v>443</v>
       </c>
@@ -10819,7 +10816,7 @@
         <v>468</v>
       </c>
       <c r="E144" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F144" s="24" t="s">
         <v>103</v>
@@ -10839,7 +10836,7 @@
         <v>470</v>
       </c>
       <c r="C145" s="29" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>471</v>
@@ -10857,7 +10854,7 @@
       <c r="K145" s="40"/>
       <c r="L145" s="20"/>
     </row>
-    <row r="146" spans="1:12" ht="50.4">
+    <row r="146" spans="1:12" ht="50.4" hidden="1">
       <c r="A146" s="4" t="s">
         <v>473</v>
       </c>
@@ -10898,7 +10895,7 @@
         <v>461</v>
       </c>
       <c r="F147" s="24" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="G147" s="6"/>
       <c r="H147" s="6"/>
@@ -10924,7 +10921,7 @@
         <v>461</v>
       </c>
       <c r="F148" s="24" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="G148" s="6"/>
       <c r="H148" s="6"/>
@@ -10950,7 +10947,7 @@
         <v>461</v>
       </c>
       <c r="F149" s="24" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="G149" s="6"/>
       <c r="H149" s="6"/>
@@ -10976,7 +10973,7 @@
         <v>461</v>
       </c>
       <c r="F150" s="24" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="G150" s="6"/>
       <c r="H150" s="6"/>
@@ -11009,7 +11006,7 @@
       <c r="K151" s="40"/>
       <c r="L151" s="20"/>
     </row>
-    <row r="152" spans="1:12" ht="84">
+    <row r="152" spans="1:12" ht="84" hidden="1">
       <c r="A152" s="4" t="s">
         <v>485</v>
       </c>
@@ -11017,7 +11014,7 @@
         <v>486</v>
       </c>
       <c r="C152" s="29" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D152" s="4" t="s">
         <v>487</v>
@@ -11026,7 +11023,7 @@
         <v>1020</v>
       </c>
       <c r="F152" s="26" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="G152" s="6"/>
       <c r="H152" s="6"/>
@@ -11035,7 +11032,7 @@
       <c r="K152" s="40"/>
       <c r="L152" s="20"/>
     </row>
-    <row r="153" spans="1:12" ht="84">
+    <row r="153" spans="1:12" ht="84" hidden="1">
       <c r="A153" s="4" t="s">
         <v>485</v>
       </c>
@@ -11043,7 +11040,7 @@
         <v>486</v>
       </c>
       <c r="C153" s="29" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D153" s="4" t="s">
         <v>487</v>
@@ -11052,7 +11049,7 @@
         <v>1020</v>
       </c>
       <c r="F153" s="26" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G153" s="6"/>
       <c r="H153" s="6"/>
@@ -11061,7 +11058,7 @@
       <c r="K153" s="40"/>
       <c r="L153" s="20"/>
     </row>
-    <row r="154" spans="1:12" ht="84">
+    <row r="154" spans="1:12" ht="84" hidden="1">
       <c r="A154" s="4" t="s">
         <v>485</v>
       </c>
@@ -11069,7 +11066,7 @@
         <v>486</v>
       </c>
       <c r="C154" s="29" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D154" s="4" t="s">
         <v>487</v>
@@ -11078,7 +11075,7 @@
         <v>1020</v>
       </c>
       <c r="F154" s="26" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G154" s="6"/>
       <c r="H154" s="6"/>
@@ -11087,7 +11084,7 @@
       <c r="K154" s="40"/>
       <c r="L154" s="20"/>
     </row>
-    <row r="155" spans="1:12" ht="84">
+    <row r="155" spans="1:12" ht="84" hidden="1">
       <c r="A155" s="4" t="s">
         <v>485</v>
       </c>
@@ -11095,7 +11092,7 @@
         <v>486</v>
       </c>
       <c r="C155" s="29" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D155" s="4" t="s">
         <v>487</v>
@@ -11104,7 +11101,7 @@
         <v>1020</v>
       </c>
       <c r="F155" s="26" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G155" s="6"/>
       <c r="H155" s="6"/>
@@ -11113,7 +11110,7 @@
       <c r="K155" s="40"/>
       <c r="L155" s="20"/>
     </row>
-    <row r="156" spans="1:12" ht="84">
+    <row r="156" spans="1:12" ht="84" hidden="1">
       <c r="A156" s="4" t="s">
         <v>485</v>
       </c>
@@ -11121,7 +11118,7 @@
         <v>486</v>
       </c>
       <c r="C156" s="29" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D156" s="4" t="s">
         <v>487</v>
@@ -11130,7 +11127,7 @@
         <v>1020</v>
       </c>
       <c r="F156" s="26" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G156" s="6"/>
       <c r="H156" s="6"/>
@@ -11139,7 +11136,7 @@
       <c r="K156" s="40"/>
       <c r="L156" s="20"/>
     </row>
-    <row r="157" spans="1:12" ht="84">
+    <row r="157" spans="1:12" ht="84" hidden="1">
       <c r="A157" s="4" t="s">
         <v>485</v>
       </c>
@@ -11147,7 +11144,7 @@
         <v>486</v>
       </c>
       <c r="C157" s="29" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="D157" s="4" t="s">
         <v>487</v>
@@ -11156,7 +11153,7 @@
         <v>1020</v>
       </c>
       <c r="F157" s="26" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="G157" s="6"/>
       <c r="H157" s="6"/>
@@ -11217,7 +11214,7 @@
         <v>496</v>
       </c>
       <c r="C160" s="30" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D160" s="4" t="s">
         <v>497</v>
@@ -11272,7 +11269,7 @@
         <v>1021</v>
       </c>
       <c r="F162" s="24" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="G162" s="6"/>
       <c r="H162" s="6"/>
@@ -11298,7 +11295,7 @@
         <v>1021</v>
       </c>
       <c r="F163" s="24" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="G163" s="6"/>
       <c r="H163" s="6"/>
@@ -11321,7 +11318,7 @@
         <v>509</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F164" s="25"/>
       <c r="G164" s="6"/>
@@ -11345,7 +11342,7 @@
         <v>513</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F165" s="24" t="s">
         <v>325</v>
@@ -11365,7 +11362,7 @@
         <v>515</v>
       </c>
       <c r="C166" s="29" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D166" t="s">
         <v>516</v>
@@ -11421,10 +11418,10 @@
         <v>524</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F168" s="24" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="G168" s="6"/>
       <c r="H168" s="6"/>
@@ -11447,10 +11444,10 @@
         <v>524</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F169" s="24" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="G169" s="6"/>
       <c r="H169" s="6"/>
@@ -11549,7 +11546,7 @@
       <c r="K173" s="40"/>
       <c r="L173" s="20"/>
     </row>
-    <row r="174" spans="1:12" ht="33.6" hidden="1">
+    <row r="174" spans="1:12" ht="33.6">
       <c r="A174" s="4" t="s">
         <v>538</v>
       </c>
@@ -11563,25 +11560,25 @@
         <v>541</v>
       </c>
       <c r="E174" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F174" s="24" t="s">
         <v>542</v>
       </c>
       <c r="G174" s="6" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H174" s="6" t="s">
         <v>1200</v>
       </c>
-      <c r="H174" s="6" t="s">
+      <c r="I174" s="33" t="s">
         <v>1201</v>
-      </c>
-      <c r="I174" s="33" t="s">
-        <v>1202</v>
       </c>
       <c r="J174" s="7"/>
       <c r="K174" s="40"/>
       <c r="L174" s="20"/>
     </row>
-    <row r="175" spans="1:12" ht="33.6" hidden="1">
+    <row r="175" spans="1:12" ht="33.6">
       <c r="A175" s="4" t="s">
         <v>538</v>
       </c>
@@ -11595,19 +11592,19 @@
         <v>541</v>
       </c>
       <c r="E175" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F175" s="24" t="s">
         <v>542</v>
       </c>
       <c r="G175" s="6" t="s">
+        <v>1202</v>
+      </c>
+      <c r="H175" s="6" t="s">
         <v>1203</v>
       </c>
-      <c r="H175" s="6" t="s">
+      <c r="I175" s="33" t="s">
         <v>1204</v>
-      </c>
-      <c r="I175" s="33" t="s">
-        <v>1205</v>
       </c>
       <c r="J175" s="7"/>
       <c r="K175" s="40"/>
@@ -12013,25 +12010,25 @@
         <v>610</v>
       </c>
       <c r="E191" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F191" s="24" t="s">
         <v>283</v>
       </c>
       <c r="G191" s="6" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H191" s="6" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I191" s="33" t="s">
         <v>1181</v>
-      </c>
-      <c r="H191" s="6" t="s">
-        <v>1183</v>
-      </c>
-      <c r="I191" s="33" t="s">
-        <v>1182</v>
       </c>
       <c r="J191" s="7"/>
       <c r="K191" s="40"/>
       <c r="L191" s="20"/>
     </row>
-    <row r="192" spans="1:12" ht="67.2">
+    <row r="192" spans="1:12" ht="67.2" hidden="1">
       <c r="C192" s="29" t="s">
         <v>611</v>
       </c>
@@ -12063,19 +12060,19 @@
         <v>616</v>
       </c>
       <c r="E193" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F193" s="24" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="G193" s="6" t="s">
         <v>617</v>
       </c>
       <c r="H193" s="6" t="s">
+        <v>1203</v>
+      </c>
+      <c r="I193" s="33" t="s">
         <v>1204</v>
-      </c>
-      <c r="I193" s="33" t="s">
-        <v>1205</v>
       </c>
       <c r="J193" s="7"/>
       <c r="K193" s="40"/>
@@ -12095,10 +12092,10 @@
         <v>616</v>
       </c>
       <c r="E194" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F194" s="24" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="G194" s="6"/>
       <c r="H194" s="6"/>
@@ -12121,10 +12118,10 @@
         <v>616</v>
       </c>
       <c r="E195" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F195" s="24" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G195" s="6"/>
       <c r="H195" s="6"/>
@@ -12147,7 +12144,7 @@
         <v>621</v>
       </c>
       <c r="E196" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F196" s="24" t="s">
         <v>622</v>
@@ -12159,7 +12156,7 @@
       <c r="K196" s="40"/>
       <c r="L196" s="20"/>
     </row>
-    <row r="197" spans="1:12" ht="33.6" hidden="1">
+    <row r="197" spans="1:12" ht="33.6">
       <c r="A197" s="4" t="s">
         <v>623</v>
       </c>
@@ -12173,7 +12170,7 @@
         <v>626</v>
       </c>
       <c r="E197" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F197" s="24" t="s">
         <v>627</v>
@@ -12225,7 +12222,7 @@
         <v>636</v>
       </c>
       <c r="E199" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F199" s="24" t="s">
         <v>637</v>
@@ -12234,7 +12231,7 @@
       <c r="H199" s="11"/>
       <c r="I199" s="34"/>
       <c r="J199" s="18" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="K199" s="41" t="s">
         <v>638</v>
@@ -12257,7 +12254,7 @@
         <v>643</v>
       </c>
       <c r="E200" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F200" s="24" t="s">
         <v>644</v>
@@ -12283,7 +12280,7 @@
         <v>648</v>
       </c>
       <c r="E201" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F201" s="24" t="s">
         <v>637</v>
@@ -12335,7 +12332,7 @@
         <v>1021</v>
       </c>
       <c r="F203" s="24" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G203" s="6"/>
       <c r="H203" s="6"/>
@@ -12358,7 +12355,7 @@
         <v>1021</v>
       </c>
       <c r="F204" s="24" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="G204" s="6"/>
       <c r="H204" s="6"/>
@@ -12381,7 +12378,7 @@
         <v>1021</v>
       </c>
       <c r="F205" s="24" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="G205" s="6"/>
       <c r="H205" s="6"/>
@@ -12404,7 +12401,7 @@
         <v>660</v>
       </c>
       <c r="E206" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F206" s="24"/>
       <c r="G206" s="6"/>
@@ -12425,7 +12422,7 @@
         <v>23</v>
       </c>
       <c r="F207" s="24" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="G207" s="6"/>
       <c r="H207" s="6"/>
@@ -12445,7 +12442,7 @@
         <v>23</v>
       </c>
       <c r="F208" s="24" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="G208" s="6"/>
       <c r="H208" s="6"/>
@@ -12486,7 +12483,7 @@
       <c r="K209" s="43"/>
       <c r="L209" s="22"/>
     </row>
-    <row r="210" spans="1:12" ht="33.6">
+    <row r="210" spans="1:12" ht="33.6" hidden="1">
       <c r="A210" s="4" t="s">
         <v>671</v>
       </c>
@@ -12524,7 +12521,7 @@
         <v>678</v>
       </c>
       <c r="E211" s="16" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F211" s="24" t="s">
         <v>679</v>
@@ -12579,7 +12576,7 @@
         <v>1021</v>
       </c>
       <c r="F213" s="24" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="G213" s="6" t="s">
         <v>689</v>
@@ -12611,7 +12608,7 @@
         <v>1021</v>
       </c>
       <c r="F214" s="24" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="G214" s="6" t="s">
         <v>689</v>
@@ -12643,7 +12640,7 @@
         <v>1021</v>
       </c>
       <c r="F215" s="24" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G215" s="6" t="s">
         <v>689</v>
@@ -12675,7 +12672,7 @@
         <v>1021</v>
       </c>
       <c r="F216" s="24" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="G216" s="6" t="s">
         <v>689</v>
@@ -12707,7 +12704,7 @@
         <v>1021</v>
       </c>
       <c r="F217" s="24" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="G217" s="6" t="s">
         <v>689</v>
@@ -12722,7 +12719,7 @@
       <c r="K217" s="40"/>
       <c r="L217" s="20"/>
     </row>
-    <row r="218" spans="1:12">
+    <row r="218" spans="1:12" hidden="1">
       <c r="A218" s="4" t="s">
         <v>692</v>
       </c>
@@ -12739,7 +12736,7 @@
         <v>1020</v>
       </c>
       <c r="F218" s="24" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="G218" s="6"/>
       <c r="H218" s="6"/>
@@ -12765,7 +12762,7 @@
         <v>1021</v>
       </c>
       <c r="F219" s="24" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="G219" s="6" t="s">
         <v>700</v>
@@ -12797,7 +12794,7 @@
         <v>1021</v>
       </c>
       <c r="F220" s="24" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="G220" s="6" t="s">
         <v>700</v>
@@ -12812,7 +12809,7 @@
       <c r="K220" s="40"/>
       <c r="L220" s="20"/>
     </row>
-    <row r="221" spans="1:12">
+    <row r="221" spans="1:12" hidden="1">
       <c r="C221" s="30" t="s">
         <v>703</v>
       </c>
@@ -12830,7 +12827,7 @@
       <c r="K221" s="40"/>
       <c r="L221" s="20"/>
     </row>
-    <row r="222" spans="1:12" ht="50.4">
+    <row r="222" spans="1:12" ht="50.4" hidden="1">
       <c r="A222" s="4" t="s">
         <v>705</v>
       </c>
@@ -12865,7 +12862,7 @@
       <c r="K223" s="40"/>
       <c r="L223" s="20"/>
     </row>
-    <row r="224" spans="1:12">
+    <row r="224" spans="1:12" hidden="1">
       <c r="A224" s="4" t="s">
         <v>709</v>
       </c>
@@ -12882,7 +12879,7 @@
         <v>1020</v>
       </c>
       <c r="F224" s="24" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G224" s="6"/>
       <c r="H224" s="6"/>
@@ -12891,7 +12888,7 @@
       <c r="K224" s="40"/>
       <c r="L224" s="20"/>
     </row>
-    <row r="225" spans="1:12">
+    <row r="225" spans="1:12" hidden="1">
       <c r="A225" s="4" t="s">
         <v>709</v>
       </c>
@@ -12908,7 +12905,7 @@
         <v>1020</v>
       </c>
       <c r="F225" s="24" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="G225" s="6"/>
       <c r="H225" s="6"/>
@@ -12917,7 +12914,7 @@
       <c r="K225" s="40"/>
       <c r="L225" s="20"/>
     </row>
-    <row r="226" spans="1:12">
+    <row r="226" spans="1:12" hidden="1">
       <c r="A226" s="4" t="s">
         <v>709</v>
       </c>
@@ -12934,7 +12931,7 @@
         <v>1020</v>
       </c>
       <c r="F226" s="24" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="G226" s="6"/>
       <c r="H226" s="6"/>
@@ -12943,7 +12940,7 @@
       <c r="K226" s="40"/>
       <c r="L226" s="20"/>
     </row>
-    <row r="227" spans="1:12">
+    <row r="227" spans="1:12" hidden="1">
       <c r="A227" s="4" t="s">
         <v>709</v>
       </c>
@@ -12960,7 +12957,7 @@
         <v>1020</v>
       </c>
       <c r="F227" s="24" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="G227" s="6"/>
       <c r="H227" s="6"/>
@@ -12995,7 +12992,7 @@
       <c r="K228" s="40"/>
       <c r="L228" s="20"/>
     </row>
-    <row r="229" spans="1:12" ht="50.4">
+    <row r="229" spans="1:12" ht="50.4" hidden="1">
       <c r="A229" s="4" t="s">
         <v>717</v>
       </c>
@@ -13012,7 +13009,7 @@
         <v>1020</v>
       </c>
       <c r="F229" s="24" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="G229" s="6"/>
       <c r="H229" s="6"/>
@@ -13021,7 +13018,7 @@
       <c r="K229" s="40"/>
       <c r="L229" s="20"/>
     </row>
-    <row r="230" spans="1:12" ht="50.4">
+    <row r="230" spans="1:12" ht="50.4" hidden="1">
       <c r="A230" s="4" t="s">
         <v>717</v>
       </c>
@@ -13038,7 +13035,7 @@
         <v>1020</v>
       </c>
       <c r="F230" s="24" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G230" s="6"/>
       <c r="H230" s="6"/>
@@ -13047,7 +13044,7 @@
       <c r="K230" s="40"/>
       <c r="L230" s="20"/>
     </row>
-    <row r="231" spans="1:12" ht="50.4">
+    <row r="231" spans="1:12" ht="50.4" hidden="1">
       <c r="A231" s="4" t="s">
         <v>717</v>
       </c>
@@ -13064,7 +13061,7 @@
         <v>1020</v>
       </c>
       <c r="F231" s="24" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="G231" s="6"/>
       <c r="H231" s="6"/>
@@ -13073,7 +13070,7 @@
       <c r="K231" s="40"/>
       <c r="L231" s="20"/>
     </row>
-    <row r="232" spans="1:12" ht="50.4">
+    <row r="232" spans="1:12" ht="50.4" hidden="1">
       <c r="A232" s="4" t="s">
         <v>717</v>
       </c>
@@ -13090,7 +13087,7 @@
         <v>1020</v>
       </c>
       <c r="F232" s="24" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G232" s="6"/>
       <c r="H232" s="6"/>
@@ -13107,7 +13104,7 @@
         <v>722</v>
       </c>
       <c r="C233" s="29" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D233" s="4" t="s">
         <v>723</v>
@@ -13139,19 +13136,19 @@
         <v>728</v>
       </c>
       <c r="E234" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F234" s="24" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G234" s="6" t="s">
+        <v>1196</v>
+      </c>
+      <c r="H234" s="6" t="s">
         <v>1197</v>
       </c>
-      <c r="H234" s="6" t="s">
+      <c r="I234" s="33" t="s">
         <v>1198</v>
-      </c>
-      <c r="I234" s="33" t="s">
-        <v>1199</v>
       </c>
       <c r="J234" s="7"/>
       <c r="K234" s="40"/>
@@ -13171,19 +13168,19 @@
         <v>728</v>
       </c>
       <c r="E235" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F235" s="24" t="s">
         <v>71</v>
       </c>
       <c r="G235" s="6" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H235" s="6" t="s">
         <v>1174</v>
       </c>
-      <c r="H235" s="6" t="s">
+      <c r="I235" s="33" t="s">
         <v>1175</v>
-      </c>
-      <c r="I235" s="33" t="s">
-        <v>1176</v>
       </c>
       <c r="J235" s="7"/>
       <c r="K235" s="40"/>
@@ -13236,7 +13233,7 @@
       <c r="H237" s="11"/>
       <c r="I237" s="34"/>
       <c r="J237" s="18" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="K237" s="41" t="s">
         <v>738</v>
@@ -13245,7 +13242,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="238" spans="1:12">
+    <row r="238" spans="1:12" hidden="1">
       <c r="A238" s="4" t="s">
         <v>740</v>
       </c>
@@ -13277,7 +13274,7 @@
         <v>745</v>
       </c>
       <c r="E239" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F239" s="25"/>
       <c r="G239" s="6"/>
@@ -13304,7 +13301,7 @@
         <v>750</v>
       </c>
       <c r="F240" s="24" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="G240" s="6"/>
       <c r="H240" s="6"/>
@@ -13330,7 +13327,7 @@
         <v>750</v>
       </c>
       <c r="F241" s="24" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="G241" s="6"/>
       <c r="H241" s="6"/>
@@ -13363,7 +13360,7 @@
       <c r="K242" s="40"/>
       <c r="L242" s="20"/>
     </row>
-    <row r="243" spans="1:12" ht="33.6">
+    <row r="243" spans="1:12" ht="33.6" hidden="1">
       <c r="A243" s="4" t="s">
         <v>755</v>
       </c>
@@ -13397,7 +13394,7 @@
         <v>761</v>
       </c>
       <c r="E244" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F244" s="24" t="s">
         <v>762</v>
@@ -13426,7 +13423,7 @@
         <v>1021</v>
       </c>
       <c r="F245" s="24" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="G245" s="6"/>
       <c r="H245" s="6"/>
@@ -13452,7 +13449,7 @@
         <v>1021</v>
       </c>
       <c r="F246" s="24" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="G246" s="6"/>
       <c r="H246" s="6"/>
@@ -13475,7 +13472,7 @@
         <v>770</v>
       </c>
       <c r="E247" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F247" s="24" t="s">
         <v>103</v>
@@ -13495,7 +13492,7 @@
         <v>772</v>
       </c>
       <c r="C248" s="29" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D248" t="s">
         <v>773</v>
@@ -13513,7 +13510,7 @@
       <c r="K248" s="40"/>
       <c r="L248" s="20"/>
     </row>
-    <row r="249" spans="1:12">
+    <row r="249" spans="1:12" hidden="1">
       <c r="A249" s="4" t="s">
         <v>775</v>
       </c>
@@ -13537,7 +13534,7 @@
       <c r="K249" s="40"/>
       <c r="L249" s="20"/>
     </row>
-    <row r="250" spans="1:12" ht="67.2">
+    <row r="250" spans="1:12" ht="67.2" hidden="1">
       <c r="A250" s="4" t="s">
         <v>779</v>
       </c>
@@ -13563,7 +13560,7 @@
       <c r="K250" s="40"/>
       <c r="L250" s="20"/>
     </row>
-    <row r="251" spans="1:12" ht="50.4">
+    <row r="251" spans="1:12" ht="50.4" hidden="1">
       <c r="A251" s="4" t="s">
         <v>784</v>
       </c>
@@ -13624,10 +13621,10 @@
         <v>795</v>
       </c>
       <c r="E253" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F253" s="24" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="G253" s="6"/>
       <c r="H253" s="6"/>
@@ -13650,10 +13647,10 @@
         <v>795</v>
       </c>
       <c r="E254" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F254" s="24" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="G254" s="6"/>
       <c r="H254" s="6"/>
@@ -13662,7 +13659,7 @@
       <c r="K254" s="40"/>
       <c r="L254" s="20"/>
     </row>
-    <row r="255" spans="1:12">
+    <row r="255" spans="1:12" hidden="1">
       <c r="A255" s="4" t="s">
         <v>796</v>
       </c>
@@ -13699,10 +13696,10 @@
         <v>803</v>
       </c>
       <c r="E256" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F256" s="24" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="G256" s="6"/>
       <c r="H256" s="6"/>
@@ -13725,7 +13722,7 @@
         <v>803</v>
       </c>
       <c r="E257" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F257" s="24" t="s">
         <v>71</v>
@@ -13745,7 +13742,7 @@
         <v>805</v>
       </c>
       <c r="C258" s="29" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D258" t="s">
         <v>806</v>
@@ -13777,7 +13774,7 @@
         <v>811</v>
       </c>
       <c r="E259" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F259" s="24" t="s">
         <v>812</v>
@@ -13832,7 +13829,7 @@
         <v>1021</v>
       </c>
       <c r="F261" s="24" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G261" s="6"/>
       <c r="H261" s="6"/>
@@ -13858,7 +13855,7 @@
         <v>1021</v>
       </c>
       <c r="F262" s="24" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="G262" s="6"/>
       <c r="H262" s="6"/>
@@ -13884,7 +13881,7 @@
         <v>1021</v>
       </c>
       <c r="F263" s="24" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="G263" s="6"/>
       <c r="H263" s="6"/>
@@ -13910,7 +13907,7 @@
         <v>1021</v>
       </c>
       <c r="F264" s="24" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="G264" s="6"/>
       <c r="H264" s="6"/>
@@ -13936,7 +13933,7 @@
         <v>1021</v>
       </c>
       <c r="F265" s="24" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="G265" s="6"/>
       <c r="H265" s="6"/>
@@ -13945,7 +13942,7 @@
       <c r="K265" s="40"/>
       <c r="L265" s="20"/>
     </row>
-    <row r="266" spans="1:12">
+    <row r="266" spans="1:12" hidden="1">
       <c r="A266" s="4" t="s">
         <v>822</v>
       </c>
@@ -13953,7 +13950,7 @@
         <v>823</v>
       </c>
       <c r="C266" s="29" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D266" s="4" t="s">
         <v>824</v>
@@ -13962,7 +13959,7 @@
         <v>1020</v>
       </c>
       <c r="F266" s="24" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="G266" s="6"/>
       <c r="H266" s="6"/>
@@ -13971,7 +13968,7 @@
       <c r="K266" s="40"/>
       <c r="L266" s="20"/>
     </row>
-    <row r="267" spans="1:12">
+    <row r="267" spans="1:12" hidden="1">
       <c r="A267" s="4" t="s">
         <v>822</v>
       </c>
@@ -13979,7 +13976,7 @@
         <v>823</v>
       </c>
       <c r="C267" s="29" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D267" s="4" t="s">
         <v>824</v>
@@ -13997,7 +13994,7 @@
       <c r="K267" s="40"/>
       <c r="L267" s="20"/>
     </row>
-    <row r="268" spans="1:12">
+    <row r="268" spans="1:12" hidden="1">
       <c r="A268" s="4" t="s">
         <v>822</v>
       </c>
@@ -14005,7 +14002,7 @@
         <v>823</v>
       </c>
       <c r="C268" s="29" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D268" s="4" t="s">
         <v>824</v>
@@ -14031,7 +14028,7 @@
         <v>826</v>
       </c>
       <c r="C269" s="29" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D269" s="4" t="s">
         <v>827</v>
@@ -14047,7 +14044,7 @@
       <c r="K269" s="40"/>
       <c r="L269" s="20"/>
     </row>
-    <row r="270" spans="1:12" ht="33.6" hidden="1">
+    <row r="270" spans="1:12" ht="33.6">
       <c r="A270" s="4" t="s">
         <v>828</v>
       </c>
@@ -14061,7 +14058,7 @@
         <v>831</v>
       </c>
       <c r="E270" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F270" s="25"/>
       <c r="G270" s="6"/>
@@ -14085,16 +14082,16 @@
         <v>835</v>
       </c>
       <c r="E271" s="16" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F271" s="24" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="G271" s="6"/>
       <c r="H271" s="6"/>
       <c r="I271" s="34"/>
       <c r="J271" s="18" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="K271" s="41" t="s">
         <v>836</v>
@@ -14126,13 +14123,13 @@
       <c r="H272" s="11"/>
       <c r="I272" s="34"/>
       <c r="J272" s="18" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="K272" s="41" t="s">
+        <v>1205</v>
+      </c>
+      <c r="L272" s="20" t="s">
         <v>1206</v>
-      </c>
-      <c r="L272" s="20" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="273" spans="1:12" ht="84" hidden="1">
@@ -14158,13 +14155,13 @@
       <c r="H273" s="11"/>
       <c r="I273" s="34"/>
       <c r="J273" s="18" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="K273" s="41" t="s">
+        <v>1207</v>
+      </c>
+      <c r="L273" s="20" t="s">
         <v>1208</v>
-      </c>
-      <c r="L273" s="20" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="274" spans="1:12" ht="84" hidden="1">
@@ -14190,13 +14187,13 @@
       <c r="H274" s="11"/>
       <c r="I274" s="34"/>
       <c r="J274" s="18" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="K274" s="41" t="s">
+        <v>1209</v>
+      </c>
+      <c r="L274" s="20" t="s">
         <v>1210</v>
-      </c>
-      <c r="L274" s="20" t="s">
-        <v>1211</v>
       </c>
     </row>
     <row r="275" spans="1:12" ht="84" hidden="1">
@@ -14222,13 +14219,13 @@
       <c r="H275" s="11"/>
       <c r="I275" s="34"/>
       <c r="J275" s="18" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="K275" s="41" t="s">
+        <v>1211</v>
+      </c>
+      <c r="L275" s="20" t="s">
         <v>1212</v>
-      </c>
-      <c r="L275" s="20" t="s">
-        <v>1213</v>
       </c>
     </row>
     <row r="276" spans="1:12" ht="33.6" hidden="1">
@@ -14248,7 +14245,7 @@
         <v>298</v>
       </c>
       <c r="F276" s="24" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G276" s="6"/>
       <c r="H276" s="6"/>
@@ -14274,7 +14271,7 @@
         <v>298</v>
       </c>
       <c r="F277" s="24" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G277" s="6"/>
       <c r="H277" s="6"/>
@@ -14297,7 +14294,7 @@
         <v>850</v>
       </c>
       <c r="E278" s="16" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F278" s="24" t="s">
         <v>851</v>
@@ -14309,7 +14306,7 @@
       <c r="K278" s="40"/>
       <c r="L278" s="20"/>
     </row>
-    <row r="279" spans="1:12">
+    <row r="279" spans="1:12" hidden="1">
       <c r="C279" s="29" t="s">
         <v>852</v>
       </c>
@@ -14347,7 +14344,7 @@
       <c r="K280" s="40"/>
       <c r="L280" s="20"/>
     </row>
-    <row r="281" spans="1:12" ht="67.2">
+    <row r="281" spans="1:12" ht="67.2" hidden="1">
       <c r="A281" s="4" t="s">
         <v>856</v>
       </c>
@@ -14364,7 +14361,7 @@
         <v>1020</v>
       </c>
       <c r="F281" s="24" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G281" s="6"/>
       <c r="H281" s="6"/>
@@ -14373,7 +14370,7 @@
       <c r="K281" s="40"/>
       <c r="L281" s="20"/>
     </row>
-    <row r="282" spans="1:12" ht="67.2">
+    <row r="282" spans="1:12" ht="67.2" hidden="1">
       <c r="A282" s="4" t="s">
         <v>856</v>
       </c>
@@ -14390,7 +14387,7 @@
         <v>1020</v>
       </c>
       <c r="F282" s="24" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G282" s="6"/>
       <c r="H282" s="6"/>
@@ -14399,7 +14396,7 @@
       <c r="K282" s="40"/>
       <c r="L282" s="20"/>
     </row>
-    <row r="283" spans="1:12" ht="67.2">
+    <row r="283" spans="1:12" ht="67.2" hidden="1">
       <c r="A283" s="4" t="s">
         <v>856</v>
       </c>
@@ -14416,7 +14413,7 @@
         <v>1020</v>
       </c>
       <c r="F283" s="24" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G283" s="6"/>
       <c r="H283" s="6"/>
@@ -14425,7 +14422,7 @@
       <c r="K283" s="40"/>
       <c r="L283" s="20"/>
     </row>
-    <row r="284" spans="1:12" ht="50.4">
+    <row r="284" spans="1:12" ht="50.4" hidden="1">
       <c r="A284" s="4" t="s">
         <v>740</v>
       </c>
@@ -14442,7 +14439,7 @@
         <v>1020</v>
       </c>
       <c r="F284" s="24" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G284" s="6"/>
       <c r="H284" s="6"/>
@@ -14451,7 +14448,7 @@
       <c r="K284" s="40"/>
       <c r="L284" s="20"/>
     </row>
-    <row r="285" spans="1:12" ht="50.4">
+    <row r="285" spans="1:12" ht="50.4" hidden="1">
       <c r="A285" s="4" t="s">
         <v>740</v>
       </c>
@@ -14468,7 +14465,7 @@
         <v>1020</v>
       </c>
       <c r="F285" s="24" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G285" s="6"/>
       <c r="H285" s="6"/>
@@ -14477,7 +14474,7 @@
       <c r="K285" s="40"/>
       <c r="L285" s="20"/>
     </row>
-    <row r="286" spans="1:12" ht="50.4">
+    <row r="286" spans="1:12" ht="50.4" hidden="1">
       <c r="A286" s="4" t="s">
         <v>740</v>
       </c>
@@ -14494,7 +14491,7 @@
         <v>1020</v>
       </c>
       <c r="F286" s="24" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G286" s="6"/>
       <c r="H286" s="6"/>
@@ -14503,7 +14500,7 @@
       <c r="K286" s="40"/>
       <c r="L286" s="20"/>
     </row>
-    <row r="287" spans="1:12" ht="50.4">
+    <row r="287" spans="1:12" ht="50.4" hidden="1">
       <c r="A287" s="4" t="s">
         <v>740</v>
       </c>
@@ -14520,7 +14517,7 @@
         <v>1020</v>
       </c>
       <c r="F287" s="24" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G287" s="6"/>
       <c r="H287" s="6"/>
@@ -14529,7 +14526,7 @@
       <c r="K287" s="40"/>
       <c r="L287" s="20"/>
     </row>
-    <row r="288" spans="1:12" ht="50.4">
+    <row r="288" spans="1:12" ht="50.4" hidden="1">
       <c r="A288" s="4" t="s">
         <v>740</v>
       </c>
@@ -14546,7 +14543,7 @@
         <v>1020</v>
       </c>
       <c r="F288" s="24" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G288" s="6"/>
       <c r="H288" s="6"/>
@@ -14555,7 +14552,7 @@
       <c r="K288" s="40"/>
       <c r="L288" s="20"/>
     </row>
-    <row r="289" spans="1:12">
+    <row r="289" spans="1:12" hidden="1">
       <c r="A289" s="4" t="s">
         <v>862</v>
       </c>
@@ -14589,7 +14586,7 @@
         <v>868</v>
       </c>
       <c r="C290" s="29" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D290" t="s">
         <v>869</v>
@@ -14607,7 +14604,7 @@
       <c r="K290" s="40"/>
       <c r="L290" s="20"/>
     </row>
-    <row r="291" spans="1:12" hidden="1">
+    <row r="291" spans="1:12">
       <c r="A291" s="4" t="s">
         <v>871</v>
       </c>
@@ -14615,13 +14612,13 @@
         <v>872</v>
       </c>
       <c r="C291" s="29" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D291" t="s">
         <v>873</v>
       </c>
       <c r="E291" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F291" s="24" t="s">
         <v>874</v>
@@ -14633,7 +14630,7 @@
       <c r="K291" s="40"/>
       <c r="L291" s="20"/>
     </row>
-    <row r="292" spans="1:12" hidden="1">
+    <row r="292" spans="1:12">
       <c r="A292" s="4" t="s">
         <v>875</v>
       </c>
@@ -14641,13 +14638,13 @@
         <v>876</v>
       </c>
       <c r="C292" s="29" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D292" t="s">
         <v>877</v>
       </c>
       <c r="E292" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F292" s="24" t="s">
         <v>878</v>
@@ -14667,13 +14664,13 @@
         <v>880</v>
       </c>
       <c r="C293" s="29" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D293" s="4" t="s">
         <v>881</v>
       </c>
       <c r="E293" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F293" s="24" t="s">
         <v>882</v>
@@ -14685,7 +14682,7 @@
       <c r="K293" s="40"/>
       <c r="L293" s="20"/>
     </row>
-    <row r="294" spans="1:12">
+    <row r="294" spans="1:12" hidden="1">
       <c r="A294" s="4" t="s">
         <v>883</v>
       </c>
@@ -14723,7 +14720,7 @@
         <v>890</v>
       </c>
       <c r="E295" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F295" s="24" t="s">
         <v>891</v>
@@ -14749,7 +14746,7 @@
         <v>895</v>
       </c>
       <c r="E296" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F296" s="24" t="s">
         <v>896</v>
@@ -14761,7 +14758,7 @@
       <c r="K296" s="43"/>
       <c r="L296" s="22"/>
     </row>
-    <row r="297" spans="1:12" hidden="1">
+    <row r="297" spans="1:12">
       <c r="A297" s="4" t="s">
         <v>897</v>
       </c>
@@ -14769,13 +14766,13 @@
         <v>898</v>
       </c>
       <c r="C297" s="29" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D297" t="s">
         <v>899</v>
       </c>
       <c r="E297" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F297" s="24" t="s">
         <v>900</v>
@@ -14801,7 +14798,7 @@
         <v>904</v>
       </c>
       <c r="E298" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F298" s="25"/>
       <c r="G298" s="6"/>
@@ -14819,7 +14816,7 @@
         <v>906</v>
       </c>
       <c r="C299" s="29" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D299" s="4" t="s">
         <v>907</v>
@@ -14887,7 +14884,7 @@
         <v>895</v>
       </c>
       <c r="E302" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F302" s="24" t="s">
         <v>916</v>
@@ -14899,7 +14896,7 @@
       <c r="K302" s="40"/>
       <c r="L302" s="20"/>
     </row>
-    <row r="303" spans="1:12" ht="33.6" hidden="1">
+    <row r="303" spans="1:12" ht="33.6">
       <c r="C303" s="29" t="s">
         <v>917</v>
       </c>
@@ -14907,7 +14904,7 @@
         <v>918</v>
       </c>
       <c r="E303" s="15" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F303" s="24" t="s">
         <v>919</v>
@@ -15003,7 +15000,7 @@
         <v>935</v>
       </c>
       <c r="E307" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F307" s="24" t="s">
         <v>103</v>
@@ -15015,7 +15012,7 @@
       <c r="K307" s="40"/>
       <c r="L307" s="20"/>
     </row>
-    <row r="308" spans="1:12" ht="33.6">
+    <row r="308" spans="1:12" ht="33.6" hidden="1">
       <c r="A308" s="4" t="s">
         <v>936</v>
       </c>
@@ -15039,7 +15036,7 @@
       <c r="K308" s="40"/>
       <c r="L308" s="20"/>
     </row>
-    <row r="309" spans="1:12" ht="33.6">
+    <row r="309" spans="1:12" ht="33.6" hidden="1">
       <c r="A309" s="4" t="s">
         <v>940</v>
       </c>
@@ -15056,7 +15053,7 @@
         <v>1020</v>
       </c>
       <c r="F309" s="24" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G309" s="6"/>
       <c r="H309" s="6"/>
@@ -15065,7 +15062,7 @@
       <c r="K309" s="40"/>
       <c r="L309" s="20"/>
     </row>
-    <row r="310" spans="1:12" ht="33.6">
+    <row r="310" spans="1:12" ht="33.6" hidden="1">
       <c r="A310" s="4" t="s">
         <v>940</v>
       </c>
@@ -15082,7 +15079,7 @@
         <v>1020</v>
       </c>
       <c r="F310" s="24" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G310" s="6"/>
       <c r="H310" s="6"/>
@@ -15091,7 +15088,7 @@
       <c r="K310" s="40"/>
       <c r="L310" s="20"/>
     </row>
-    <row r="311" spans="1:12" ht="50.4">
+    <row r="311" spans="1:12" ht="50.4" hidden="1">
       <c r="A311" s="4" t="s">
         <v>944</v>
       </c>
@@ -15167,7 +15164,7 @@
       <c r="K313" s="40"/>
       <c r="L313" s="20"/>
     </row>
-    <row r="314" spans="1:12" ht="33.6">
+    <row r="314" spans="1:12" ht="33.6" hidden="1">
       <c r="A314" s="4" t="s">
         <v>958</v>
       </c>
@@ -15231,10 +15228,10 @@
         <v>970</v>
       </c>
       <c r="E316" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F316" s="24" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="G316" s="6"/>
       <c r="H316" s="6"/>
@@ -15257,7 +15254,7 @@
         <v>970</v>
       </c>
       <c r="E317" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F317" s="24" t="s">
         <v>134</v>
@@ -15283,7 +15280,7 @@
         <v>974</v>
       </c>
       <c r="E318" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F318" s="24" t="s">
         <v>975</v>
@@ -15295,7 +15292,7 @@
       <c r="K318" s="40"/>
       <c r="L318" s="20"/>
     </row>
-    <row r="319" spans="1:12">
+    <row r="319" spans="1:12" hidden="1">
       <c r="A319" s="4" t="s">
         <v>976</v>
       </c>
@@ -15312,12 +15309,12 @@
         <v>1020</v>
       </c>
       <c r="F319" s="24" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="K319" s="40"/>
       <c r="L319" s="20"/>
     </row>
-    <row r="320" spans="1:12">
+    <row r="320" spans="1:12" hidden="1">
       <c r="A320" s="4" t="s">
         <v>976</v>
       </c>
@@ -15334,22 +15331,22 @@
         <v>1020</v>
       </c>
       <c r="F320" s="24" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="G320" s="6" t="s">
+        <v>1214</v>
+      </c>
+      <c r="H320" s="6" t="s">
         <v>1215</v>
       </c>
-      <c r="H320" s="6" t="s">
-        <v>1216</v>
-      </c>
       <c r="I320" s="38" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="J320" s="17"/>
       <c r="K320" s="40"/>
       <c r="L320" s="20"/>
     </row>
-    <row r="321" spans="1:12">
+    <row r="321" spans="1:12" hidden="1">
       <c r="A321" s="4" t="s">
         <v>976</v>
       </c>
@@ -15366,7 +15363,7 @@
         <v>1020</v>
       </c>
       <c r="F321" s="24" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="G321" s="6"/>
       <c r="H321" s="6"/>
@@ -15375,7 +15372,7 @@
       <c r="K321" s="40"/>
       <c r="L321" s="20"/>
     </row>
-    <row r="322" spans="1:12">
+    <row r="322" spans="1:12" hidden="1">
       <c r="A322" s="4" t="s">
         <v>976</v>
       </c>
@@ -15392,7 +15389,7 @@
         <v>1020</v>
       </c>
       <c r="F322" s="24" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="G322" s="6"/>
       <c r="H322" s="6"/>
@@ -15401,7 +15398,7 @@
       <c r="K322" s="40"/>
       <c r="L322" s="20"/>
     </row>
-    <row r="323" spans="1:12">
+    <row r="323" spans="1:12" hidden="1">
       <c r="A323" s="4" t="s">
         <v>976</v>
       </c>
@@ -15418,7 +15415,7 @@
         <v>1020</v>
       </c>
       <c r="F323" s="24" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="G323" s="6"/>
       <c r="H323" s="6"/>
@@ -15427,7 +15424,7 @@
       <c r="K323" s="40"/>
       <c r="L323" s="20"/>
     </row>
-    <row r="324" spans="1:12">
+    <row r="324" spans="1:12" hidden="1">
       <c r="A324" s="4" t="s">
         <v>976</v>
       </c>
@@ -15444,7 +15441,7 @@
         <v>1020</v>
       </c>
       <c r="F324" s="24" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="G324" s="6"/>
       <c r="H324" s="6"/>
@@ -15467,7 +15464,7 @@
         <v>983</v>
       </c>
       <c r="E325" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F325" s="24" t="s">
         <v>984</v>
@@ -15493,7 +15490,7 @@
         <v>988</v>
       </c>
       <c r="E326" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F326" s="24" t="s">
         <v>637</v>
@@ -15505,7 +15502,7 @@
       <c r="K326" s="40"/>
       <c r="L326" s="20"/>
     </row>
-    <row r="327" spans="1:12" ht="50.4">
+    <row r="327" spans="1:12" ht="50.4" hidden="1">
       <c r="A327" s="4" t="s">
         <v>989</v>
       </c>
@@ -15522,7 +15519,7 @@
         <v>1020</v>
       </c>
       <c r="F327" s="24" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="G327" s="6"/>
       <c r="H327" s="6"/>
@@ -15531,7 +15528,7 @@
       <c r="K327" s="40"/>
       <c r="L327" s="20"/>
     </row>
-    <row r="328" spans="1:12" ht="50.4">
+    <row r="328" spans="1:12" ht="50.4" hidden="1">
       <c r="A328" s="4" t="s">
         <v>989</v>
       </c>
@@ -15557,7 +15554,7 @@
       <c r="K328" s="40"/>
       <c r="L328" s="20"/>
     </row>
-    <row r="329" spans="1:12" ht="50.4">
+    <row r="329" spans="1:12" ht="50.4" hidden="1">
       <c r="A329" s="4" t="s">
         <v>989</v>
       </c>
@@ -15574,7 +15571,7 @@
         <v>1020</v>
       </c>
       <c r="F329" s="24" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="G329" s="6"/>
       <c r="H329" s="6"/>
@@ -15623,7 +15620,7 @@
         <v>1001</v>
       </c>
       <c r="E331" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F331" s="24"/>
       <c r="G331" s="6"/>
@@ -15656,7 +15653,7 @@
       <c r="H332" s="11"/>
       <c r="I332" s="34"/>
       <c r="J332" s="18" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="K332" s="41" t="s">
         <v>1007</v>
@@ -15665,7 +15662,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="333" spans="1:12" ht="33.6" hidden="1">
+    <row r="333" spans="1:12">
       <c r="B333" t="s">
         <v>1009</v>
       </c>
@@ -15676,7 +15673,7 @@
         <v>1011</v>
       </c>
       <c r="E333" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F333" s="25"/>
       <c r="G333" s="6"/>
@@ -15703,7 +15700,7 @@
         <v>1021</v>
       </c>
       <c r="F334" s="24" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="G334" s="6"/>
       <c r="H334" s="6"/>
@@ -15729,7 +15726,7 @@
         <v>1021</v>
       </c>
       <c r="F335" s="24" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="G335" s="6"/>
       <c r="H335" s="6"/>
@@ -15755,7 +15752,7 @@
         <v>1021</v>
       </c>
       <c r="F336" s="24" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="G336" s="6"/>
       <c r="H336" s="6"/>
@@ -15781,7 +15778,7 @@
         <v>1021</v>
       </c>
       <c r="F337" s="24" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="G337" s="6"/>
       <c r="H337" s="6"/>
@@ -15807,7 +15804,7 @@
         <v>1021</v>
       </c>
       <c r="F338" s="24" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="G338" s="6"/>
       <c r="H338" s="6"/>
@@ -15820,7 +15817,7 @@
   <autoFilter ref="E1:E338" xr:uid="{400770C2-249E-0F45-890C-AF972D0CDD11}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Other"/>
+        <filter val="X-linked dominant"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>